<commit_message>
checkpoint: refactored through filter and trim
</commit_message>
<xml_diff>
--- a/test/sample-information.xlsx
+++ b/test/sample-information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhoffman/src/dada2-nf/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhoffman/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3E3064C-FC28-0E4F-A008-E6B2EF7A95C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA22859-494B-974E-B0DB-E4DEE33B7C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample-information" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>sampleid</t>
   </si>
@@ -65,12 +65,6 @@
   </si>
   <si>
     <t>s505</t>
-  </si>
-  <si>
-    <t>m3n701-s506</t>
-  </si>
-  <si>
-    <t>s506</t>
   </si>
   <si>
     <t>m3n714-s510</t>
@@ -130,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -964,8 +958,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1067,34 +1061,37 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>12434</v>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1103,30 +1100,27 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
         <v>23</v>
       </c>
+      <c r="B7">
+        <v>18992</v>
+      </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1137,10 +1131,10 @@
         <v>18992</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -1151,16 +1145,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>19137</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="B9">
-        <v>18992</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1173,50 +1167,30 @@
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
-        <v>19137</v>
+      <c r="B10" t="s">
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10">
         <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
       <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
         <v>2</v>
       </c>
     </row>

</xml_diff>